<commit_message>
Updating the test data for PROD environment
</commit_message>
<xml_diff>
--- a/Testdata/DataFile_LiveSLR_PROD.xlsx
+++ b/Testdata/DataFile_LiveSLR_PROD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CE116-7555-48B9-B03F-60B08C7932F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBDCD22-7CA1-4999-A8B0-4FD6E3228D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Population</t>
   </si>
@@ -262,48 +262,6 @@
     <t>Real-world Evidence_radio_button</t>
   </si>
   <si>
-    <t>Interventional</t>
-  </si>
-  <si>
-    <t>Interventional_radio_button</t>
-  </si>
-  <si>
-    <t>WordReport-Pfizer - MM RRMM-Interventional-</t>
-  </si>
-  <si>
-    <t>ExcelReport-Pfizer - MM RRMM-Economic-</t>
-  </si>
-  <si>
-    <t>WordReport-Pfizer - MM RRMM-Economic-</t>
-  </si>
-  <si>
-    <t>ExcelReport-Pfizer - MM RRMM-Quality of Life-</t>
-  </si>
-  <si>
-    <t>WordReport-Pfizer - MM RRMM-Quality of Life-</t>
-  </si>
-  <si>
-    <t>ExcelReport-Pfizer - MM RRMM-Real-world Evidence-</t>
-  </si>
-  <si>
-    <t>WordReport-Pfizer - MM RRMM-Real-world Evidence-</t>
-  </si>
-  <si>
-    <t>Pfizer - MM Maintenance</t>
-  </si>
-  <si>
-    <t>Pfizer - MM Maintenance_radio_button</t>
-  </si>
-  <si>
-    <t>ExcelReport-Pfizer - MM Main-Interventional</t>
-  </si>
-  <si>
-    <t>ExcelReport-Pfizer - MM Maintenance-Interventional-</t>
-  </si>
-  <si>
-    <t>WordReport-Pfizer - MM Maintenance-Interventional-</t>
-  </si>
-  <si>
     <t>ExcelReport-Pfizer - MM Maintenance-Economic-</t>
   </si>
   <si>
@@ -320,6 +278,54 @@
   </si>
   <si>
     <t>WordReport-Pfizer - MM Maintenance-Real-world Evidence-</t>
+  </si>
+  <si>
+    <t>Clinical</t>
+  </si>
+  <si>
+    <t>Clinical_radio_button</t>
+  </si>
+  <si>
+    <t>ExcelReport-Pfizer - MM Maintenance-Clinical-</t>
+  </si>
+  <si>
+    <t>WordReport-Pfizer - MM Maintenance-Clinical-</t>
+  </si>
+  <si>
+    <t>Takeda - MM Maintenance</t>
+  </si>
+  <si>
+    <t>Takeda - MM Maintenance_radio_button</t>
+  </si>
+  <si>
+    <t>ExpectedSourceTemplateFile</t>
+  </si>
+  <si>
+    <t>ExcelReport-Takeda - MM Maintenance-Clinical-</t>
+  </si>
+  <si>
+    <t>WordReport-Takeda - MM Maintenance-Clinical-</t>
+  </si>
+  <si>
+    <t>ExcelReport-Takeda - MM Maintenance-Economic-</t>
+  </si>
+  <si>
+    <t>ExcelReport-Takeda - MM Maintenance-Quality of Life-</t>
+  </si>
+  <si>
+    <t>ExcelReport-Takeda - MM Maintenance-Real-world Evidence-</t>
+  </si>
+  <si>
+    <t>WordReport-Takeda - MM Maintenance-Economic-</t>
+  </si>
+  <si>
+    <t>WordReport-Takeda - MM Maintenance-Quality of Life-</t>
+  </si>
+  <si>
+    <t>WordReport-Takeda - MM Maintenance-Real-world Evidence-</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\SLRReport_SourceData\PROD_Data\Expected_Source_Data_Manipulated.xlsx</t>
   </si>
 </sst>
 </file>
@@ -637,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,12 +659,13 @@
     <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -684,27 +691,30 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -719,16 +729,19 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>69</v>
       </c>
@@ -747,17 +760,17 @@
       <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
-        <v>86</v>
-      </c>
       <c r="J3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>71</v>
       </c>
@@ -776,17 +789,17 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
-        <v>77</v>
-      </c>
       <c r="J4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>73</v>
       </c>
@@ -805,203 +818,203 @@
       <c r="H5" t="s">
         <v>32</v>
       </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
       <c r="J5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>35</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
         <v>79</v>
       </c>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I7" t="s">
+      <c r="K17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
         <v>80</v>
       </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I12" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
-        <v>89</v>
-      </c>
-      <c r="J13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I15" t="s">
-        <v>91</v>
-      </c>
-      <c r="J15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I16" t="s">
-        <v>92</v>
-      </c>
-      <c r="J16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I17" t="s">
-        <v>93</v>
-      </c>
-      <c r="J17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J19" t="s">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J20" t="s">
+    <row r="20" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J21" t="s">
+    <row r="21" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J22" t="s">
+    <row r="22" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J23" t="s">
+    <row r="23" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J24" t="s">
+    <row r="24" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J25" t="s">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J26" t="s">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J27" t="s">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J28" t="s">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J29" t="s">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J30" t="s">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="J31" t="s">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>